<commit_message>
update tool import areas
</commit_message>
<xml_diff>
--- a/engines/gns_area/database/danh_sach_cap_tinh_2019_02_28.xlsx
+++ b/engines/gns_area/database/danh_sach_cap_tinh_2019_02_28.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Việt Nam #1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -225,7 +225,7 @@
     <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -551,7 +551,7 @@
   <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M55" sqref="M55"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>